<commit_message>
att ordenação da coluna ano para cálculo do índice deflator
</commit_message>
<xml_diff>
--- a/Data/g9.1.xlsx
+++ b/Data/g9.1.xlsx
@@ -468,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/12/2010</t>
+          <t>01/12/2009</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10.09174311926606</v>
+        <v>-9.166666666666668</v>
       </c>
     </row>
     <row r="3">
@@ -488,11 +488,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/12/2011</t>
+          <t>01/12/2010</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5.952380952380953</v>
+        <v>-5.61797752808989</v>
       </c>
     </row>
     <row r="4">
@@ -508,11 +508,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/12/2012</t>
+          <t>01/12/2011</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6.853932584269651</v>
+        <v>-6.414300736067291</v>
       </c>
     </row>
     <row r="5">
@@ -528,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/12/2013</t>
+          <t>01/12/2012</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5.467928496319674</v>
+        <v>-5.184446660019947</v>
       </c>
     </row>
     <row r="6">
@@ -548,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/12/2014</t>
+          <t>01/12/2013</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-0.3988035892322994</v>
+        <v>0.4004004004003914</v>
       </c>
     </row>
     <row r="7">
@@ -568,11 +568,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/12/2015</t>
+          <t>01/12/2014</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-7.207207207207212</v>
+        <v>7.766990291262132</v>
       </c>
     </row>
     <row r="8">
@@ -588,11 +588,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/12/2016</t>
+          <t>01/12/2015</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-5.82524271844661</v>
+        <v>6.185567010309279</v>
       </c>
     </row>
     <row r="9">
@@ -608,11 +608,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/12/2017</t>
+          <t>01/12/2016</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5.612829324169533</v>
+        <v>-5.314533622559658</v>
       </c>
     </row>
     <row r="10">
@@ -628,11 +628,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/12/2018</t>
+          <t>01/12/2017</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1.518438177874182</v>
+        <v>-1.49572649572649</v>
       </c>
     </row>
     <row r="11">
@@ -648,11 +648,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01/12/2019</t>
+          <t>01/12/2018</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4.380341880341887</v>
+        <v>-4.196519959058353</v>
       </c>
     </row>
     <row r="12">
@@ -668,11 +668,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01/12/2020</t>
+          <t>01/12/2019</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.5117707267144223</v>
+        <v>-0.5091649694501044</v>
       </c>
     </row>
     <row r="13">
@@ -688,11 +688,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01/12/2021</t>
+          <t>01/12/2020</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-2.851323828920571</v>
+        <v>2.9350104821803</v>
       </c>
     </row>
     <row r="14">
@@ -708,11 +708,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01/12/2010</t>
+          <t>01/12/2009</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10.61906913691821</v>
+        <v>-9.599673202614378</v>
       </c>
     </row>
     <row r="15">
@@ -728,11 +728,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01/12/2011</t>
+          <t>01/12/2010</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.47385620915033</v>
+        <v>-5.189775367931837</v>
       </c>
     </row>
     <row r="16">
@@ -748,11 +748,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/12/2012</t>
+          <t>01/12/2011</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8.068680609346778</v>
+        <v>-7.466252538525875</v>
       </c>
     </row>
     <row r="17">
@@ -768,11 +768,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/12/2013</t>
+          <t>01/12/2012</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7.322900489786166</v>
+        <v>-6.823241317898477</v>
       </c>
     </row>
     <row r="18">
@@ -788,11 +788,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/12/2014</t>
+          <t>01/12/2013</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.7902938557435513</v>
+        <v>0.7965892516548889</v>
       </c>
     </row>
     <row r="19">
@@ -808,11 +808,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/12/2015</t>
+          <t>01/12/2014</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>-9.39077751598788</v>
+        <v>10.36404160475484</v>
       </c>
     </row>
     <row r="20">
@@ -828,11 +828,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/12/2016</t>
+          <t>01/12/2015</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-5.819712729073789</v>
+        <v>6.179332106231916</v>
       </c>
     </row>
     <row r="21">
@@ -848,11 +848,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/12/2017</t>
+          <t>01/12/2016</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3.15540362871416</v>
+        <v>-3.05888350751975</v>
       </c>
     </row>
     <row r="22">
@@ -868,11 +868,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01/12/2018</t>
+          <t>01/12/2017</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.2549069589599773</v>
+        <v>-0.2542588354945363</v>
       </c>
     </row>
     <row r="23">
@@ -888,11 +888,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01/12/2019</t>
+          <t>01/12/2018</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.114670734808023</v>
+        <v>-3.020589323141409</v>
       </c>
     </row>
     <row r="24">
@@ -908,11 +908,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01/12/2020</t>
+          <t>01/12/2019</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1.356182961410446</v>
+        <v>-1.338036735190373</v>
       </c>
     </row>
     <row r="25">
@@ -928,11 +928,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01/12/2021</t>
+          <t>01/12/2020</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-8.307991728500197</v>
+        <v>9.060758821968706</v>
       </c>
     </row>
     <row r="26">
@@ -948,11 +948,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01/12/2010</t>
+          <t>01/12/2009</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>12.48527679623086</v>
+        <v>-11.09947643979057</v>
       </c>
     </row>
     <row r="27">
@@ -968,11 +968,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01/12/2011</t>
+          <t>01/12/2010</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>-3.141361256544506</v>
+        <v>3.243243243243232</v>
       </c>
     </row>
     <row r="28">
@@ -988,11 +988,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01/12/2012</t>
+          <t>01/12/2011</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>5.081081081081074</v>
+        <v>-4.835390946502061</v>
       </c>
     </row>
     <row r="29">
@@ -1008,11 +1008,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/12/2013</t>
+          <t>01/12/2012</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.189300411522633</v>
+        <v>-3.090727816550343</v>
       </c>
     </row>
     <row r="30">
@@ -1028,11 +1028,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01/12/2014</t>
+          <t>01/12/2013</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>-0.6979062811565351</v>
+        <v>0.7028112449799284</v>
       </c>
     </row>
     <row r="31">
@@ -1048,11 +1048,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/12/2015</t>
+          <t>01/12/2014</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>-9.538152610441763</v>
+        <v>10.54384017758048</v>
       </c>
     </row>
     <row r="32">
@@ -1068,11 +1068,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01/12/2016</t>
+          <t>01/12/2015</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>-2.219755826859049</v>
+        <v>2.270147559591384</v>
       </c>
     </row>
     <row r="33">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01/12/2017</t>
+          <t>01/12/2016</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>-7.037457434733241</v>
+        <v>7.570207570207566</v>
       </c>
     </row>
     <row r="34">
@@ -1108,11 +1108,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01/12/2018</t>
+          <t>01/12/2017</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.8547008547008517</v>
+        <v>-0.8474576271186307</v>
       </c>
     </row>
     <row r="35">
@@ -1128,11 +1128,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01/12/2019</t>
+          <t>01/12/2018</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.9685230024213176</v>
+        <v>-0.9592326139088891</v>
       </c>
     </row>
     <row r="36">
@@ -1148,11 +1148,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01/12/2020</t>
+          <t>01/12/2019</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>-1.798561151079137</v>
+        <v>1.831501831501825</v>
       </c>
     </row>
     <row r="37">
@@ -1168,11 +1168,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01/12/2021</t>
+          <t>01/12/2020</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-11.47741147741148</v>
+        <v>12.96551724137931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>